<commit_message>
Updated TVS in BOM.
</commit_message>
<xml_diff>
--- a/CAM_Outputs/MAINBOARD/BOM/PrintNC_GRBLHAL_Breakout_CAM_OUTPUT_A7.xlsx
+++ b/CAM_Outputs/MAINBOARD/BOM/PrintNC_GRBLHAL_Breakout_CAM_OUTPUT_A7.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\grblhal_2000_PrintNC\Project Outputs for PrintNC_GRBLHAL_Breakout\PrintNC_GRBLHAL_Breakout_UPLOAD_GERBERS_A7\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\grblhal_2000_PrintNC\CAM_Outputs\MAINBOARD\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -308,9 +308,6 @@
     <t>SOT95P230X117-3N</t>
   </si>
   <si>
-    <t>C293966</t>
-  </si>
-  <si>
     <t>SS210</t>
   </si>
   <si>
@@ -858,6 +855,9 @@
   </si>
   <si>
     <t>C61534</t>
+  </si>
+  <si>
+    <t>C521963</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1202,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1705,7 +1707,7 @@
         <v>92</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>93</v>
+        <v>276</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
@@ -1713,19 +1715,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
@@ -1733,19 +1735,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="F27" s="1">
         <v>2</v>
@@ -1753,19 +1755,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="F28" s="1">
         <v>2</v>
@@ -1773,19 +1775,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
@@ -1793,19 +1795,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="F30" s="1">
         <v>3</v>
@@ -1813,19 +1815,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="F31" s="1">
         <v>4</v>
@@ -1833,19 +1835,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
@@ -1853,19 +1855,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="F33" s="1">
         <v>7</v>
@@ -1873,19 +1875,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
@@ -1893,19 +1895,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F35" s="1">
         <v>6</v>
@@ -1913,19 +1915,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="F36" s="1">
         <v>2</v>
@@ -1933,19 +1935,19 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="F37" s="1">
         <v>5</v>
@@ -1953,19 +1955,19 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
@@ -1973,19 +1975,19 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
@@ -1993,19 +1995,19 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="F40" s="1">
         <v>2</v>
@@ -2013,19 +2015,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
@@ -2033,19 +2035,19 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="F42" s="1">
         <v>2</v>
@@ -2053,19 +2055,19 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="F43" s="1">
         <v>1</v>
@@ -2073,19 +2075,19 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="F44" s="1">
         <v>23</v>
@@ -2093,19 +2095,19 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="F45" s="1">
         <v>3</v>
@@ -2113,19 +2115,19 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="F46" s="1">
         <v>2</v>
@@ -2133,19 +2135,19 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="F47" s="1">
         <v>14</v>
@@ -2153,19 +2155,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="F48" s="1">
         <v>15</v>
@@ -2173,19 +2175,19 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="F49" s="1">
         <v>35</v>
@@ -2193,19 +2195,19 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="F50" s="1">
         <v>8</v>
@@ -2213,19 +2215,19 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="F51" s="1">
         <v>7</v>
@@ -2233,19 +2235,19 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="F52" s="1">
         <v>15</v>
@@ -2253,19 +2255,19 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="F53" s="1">
         <v>9</v>
@@ -2273,19 +2275,19 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="F54" s="1">
         <v>5</v>
@@ -2293,19 +2295,19 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
@@ -2313,19 +2315,19 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="F56" s="1">
         <v>1</v>
@@ -2333,19 +2335,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="F57" s="1">
         <v>1</v>
@@ -2353,19 +2355,19 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="F58" s="1">
         <v>1</v>
@@ -2373,19 +2375,19 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>228</v>
       </c>
       <c r="F59" s="1">
         <v>1</v>
@@ -2393,19 +2395,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="F60" s="1">
         <v>2</v>
@@ -2413,19 +2415,19 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="F61" s="1">
         <v>15</v>
@@ -2433,19 +2435,19 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>241</v>
       </c>
       <c r="F62" s="1">
         <v>1</v>
@@ -2453,19 +2455,19 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="F63" s="1">
         <v>1</v>
@@ -2473,19 +2475,19 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="F64" s="1">
         <v>1</v>
@@ -2493,19 +2495,19 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="F65" s="1">
         <v>1</v>
@@ -2513,19 +2515,19 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>260</v>
       </c>
       <c r="F66" s="1">
         <v>1</v>
@@ -2533,19 +2535,19 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="F67" s="1">
         <v>1</v>
@@ -2553,19 +2555,19 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="D68" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="F68" s="1">
         <v>1</v>
@@ -2573,19 +2575,19 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="F69" s="1">
         <v>1</v>
@@ -2593,19 +2595,19 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="F70" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Removed teensy headers due to the fact it is hard to find teensy4.1 without headers.
</commit_message>
<xml_diff>
--- a/CAM_Outputs/MAINBOARD/BOM/PrintNC_GRBLHAL_Breakout_CAM_OUTPUT_A7.xlsx
+++ b/CAM_Outputs/MAINBOARD/BOM/PrintNC_GRBLHAL_Breakout_CAM_OUTPUT_A7.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="272">
   <si>
     <t>Comment</t>
   </si>
@@ -525,21 +525,6 @@
   </si>
   <si>
     <t>C124378</t>
-  </si>
-  <si>
-    <t>Header 24</t>
-  </si>
-  <si>
-    <t>Header, 24-Pin</t>
-  </si>
-  <si>
-    <t>P16, P17</t>
-  </si>
-  <si>
-    <t>HDR1X24</t>
-  </si>
-  <si>
-    <t>C725956</t>
   </si>
   <si>
     <t>Header 6 2mm</t>
@@ -1200,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1692,7 @@
         <v>92</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
@@ -2050,7 +2035,7 @@
         <v>170</v>
       </c>
       <c r="F42" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2064,33 +2049,33 @@
         <v>173</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="F43" s="1">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>179</v>
       </c>
       <c r="F44" s="1">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2098,216 +2083,216 @@
         <v>180</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="F45" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="F46" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F47" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F48" s="1">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F49" s="1">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F50" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F51" s="1">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F52" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F53" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F54" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
@@ -2315,19 +2300,19 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="F56" s="1">
         <v>1</v>
@@ -2335,19 +2320,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="F57" s="1">
         <v>1</v>
@@ -2355,19 +2340,19 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F58" s="1">
         <v>1</v>
@@ -2375,42 +2360,42 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F59" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>230</v>
       </c>
       <c r="F60" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2430,7 +2415,7 @@
         <v>235</v>
       </c>
       <c r="F61" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2504,10 +2489,10 @@
         <v>253</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="F65" s="1">
         <v>1</v>
@@ -2515,19 +2500,19 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>239</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F66" s="1">
         <v>1</v>
@@ -2535,19 +2520,19 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="F67" s="1">
         <v>1</v>
@@ -2555,19 +2540,19 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="D68" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="F68" s="1">
         <v>1</v>
@@ -2575,41 +2560,21 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>270</v>
       </c>
       <c r="F69" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="F70" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>